<commit_message>
added direct-comparison subset for sol/inf
</commit_message>
<xml_diff>
--- a/inputs-sequoia/genus_family.xlsx
+++ b/inputs-sequoia/genus_family.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/github/sequoia-dragen/inputs-sequoia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B14D45A-D45C-7B4B-A938-913732FC964F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED26313E-2923-FB4D-A33F-E535035BD63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="40520" windowHeight="24920" xr2:uid="{AA6A6641-1C50-7D40-AC2E-61500500FA7D}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="22400" windowHeight="25500" xr2:uid="{AA6A6641-1C50-7D40-AC2E-61500500FA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="genus_family" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Julian</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{F224526A-2393-B641-9976-69A3A07AFA0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Julian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://assets.publishing.service.gov.uk/media/67f5259ae3c60873d6c90d08/UKHSA-priority-pathogen-families-research-and-development-tool.pdf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{591C4093-A0B5-724A-8ABB-7C335ED0ECDE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Julian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://assets.publishing.service.gov.uk/media/67f5259ae3c60873d6c90d08/UKHSA-priority-pathogen-families-research-and-development-tool.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="341">
   <si>
     <t>Reporting_Name</t>
   </si>
@@ -1041,13 +1117,28 @@
   </si>
   <si>
     <t>strand.type</t>
+  </si>
+  <si>
+    <t>family_pandemic_potential</t>
+  </si>
+  <si>
+    <t>family_epidemic_potential</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1196,6 +1287,24 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
     </font>
@@ -1541,11 +1650,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1591,27 +1701,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1961,11 +2051,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB977FA-EF16-3246-B6EF-5F9C7D78C9B1}">
-  <dimension ref="A1:E243"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB977FA-EF16-3246-B6EF-5F9C7D78C9B1}">
+  <dimension ref="A1:G243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1973,9 +2063,11 @@
     <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1991,8 +2083,14 @@
       <c r="E1" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2009,7 +2107,7 @@
         <v>10804</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2025,8 +2123,14 @@
       <c r="E3" s="2">
         <v>1313215</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2042,8 +2146,14 @@
       <c r="E4" s="2">
         <v>2849717</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2059,8 +2169,14 @@
       <c r="E5" s="2">
         <v>1980456</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2076,8 +2192,14 @@
       <c r="E6" s="2">
         <v>1424613</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2093,8 +2215,14 @@
       <c r="E7" s="2">
         <v>308159</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2111,7 +2239,7 @@
         <v>90961</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -2127,8 +2255,14 @@
       <c r="E9" s="2">
         <v>3052470</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2145,7 +2279,7 @@
         <v>1891762</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2161,8 +2295,14 @@
       <c r="E11" s="2">
         <v>3052490</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2178,8 +2318,14 @@
       <c r="E12" s="2">
         <v>2010960</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -2195,8 +2341,14 @@
       <c r="E13" s="2">
         <v>1618189</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -2213,7 +2365,7 @@
         <v>565995</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -2229,8 +2381,14 @@
       <c r="E15" s="2">
         <v>80935</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -2246,8 +2404,14 @@
       <c r="E16" s="2">
         <v>35305</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -2263,8 +2427,14 @@
       <c r="E17" s="2">
         <v>1221391</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -2280,8 +2450,14 @@
       <c r="E18" s="2">
         <v>3052302</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2297,8 +2473,14 @@
       <c r="E19" s="2">
         <v>37124</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -2314,8 +2496,14 @@
       <c r="E20" s="2">
         <v>169173</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -2332,7 +2520,7 @@
         <v>46839</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -2348,8 +2536,14 @@
       <c r="E22" s="3">
         <v>42769</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -2365,8 +2559,14 @@
       <c r="E23" s="3">
         <v>12067</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -2382,8 +2582,14 @@
       <c r="E24" s="3">
         <v>42779</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -2399,8 +2605,14 @@
       <c r="E25" s="3">
         <v>12071</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -2416,8 +2628,14 @@
       <c r="E26" s="2">
         <v>3052518</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -2433,8 +2651,14 @@
       <c r="E27" s="2">
         <v>12637</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
@@ -2450,8 +2674,14 @@
       <c r="E28" s="2">
         <v>11053</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -2467,8 +2697,14 @@
       <c r="E29" s="2">
         <v>11060</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -2484,8 +2720,14 @@
       <c r="E30" s="2">
         <v>11069</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
@@ -2501,8 +2743,14 @@
       <c r="E31" s="2">
         <v>11070</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -2518,8 +2766,14 @@
       <c r="E32" s="2">
         <v>3052477</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
@@ -2536,7 +2790,7 @@
         <v>38767</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -2552,8 +2806,14 @@
       <c r="E34" s="2">
         <v>11021</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2569,8 +2829,14 @@
       <c r="E35" s="2">
         <v>1570291</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
@@ -2586,8 +2852,14 @@
       <c r="E36" s="3">
         <v>46633</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -2603,8 +2875,14 @@
       <c r="E37" s="3">
         <v>138948</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
@@ -2620,8 +2898,14 @@
       <c r="E38" s="3">
         <v>39054</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
@@ -2637,8 +2921,14 @@
       <c r="E39" s="3">
         <v>138949</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
         <v>70</v>
       </c>
@@ -2654,8 +2944,14 @@
       <c r="E40" s="3">
         <v>171720</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
@@ -2671,8 +2967,14 @@
       <c r="E41" s="3">
         <v>138950</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
@@ -2688,8 +2990,14 @@
       <c r="E42" s="3">
         <v>2650411</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
         <v>73</v>
       </c>
@@ -2705,8 +3013,14 @@
       <c r="E43" s="3">
         <v>138951</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
         <v>74</v>
       </c>
@@ -2723,7 +3037,7 @@
         <v>10376</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
         <v>77</v>
       </c>
@@ -2740,7 +3054,7 @@
         <v>38768</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
         <v>78</v>
       </c>
@@ -2756,8 +3070,14 @@
       <c r="E46" s="2">
         <v>2847089</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
         <v>79</v>
       </c>
@@ -2773,8 +3093,14 @@
       <c r="E47" s="2">
         <v>3052307</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
         <v>80</v>
       </c>
@@ -2790,8 +3116,14 @@
       <c r="E48" s="2">
         <v>3052480</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
         <v>81</v>
       </c>
@@ -2807,8 +3139,14 @@
       <c r="E49" s="2">
         <v>1216928</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
@@ -2824,8 +3162,14 @@
       <c r="E50" s="2">
         <v>3052223</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -2841,8 +3185,14 @@
       <c r="E51" s="2">
         <v>665602</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
         <v>86</v>
       </c>
@@ -2858,8 +3208,14 @@
       <c r="E52" s="2">
         <v>12092</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
         <v>88</v>
       </c>
@@ -2876,7 +3232,7 @@
         <v>10407</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
@@ -2892,8 +3248,14 @@
       <c r="E54" s="2">
         <v>3052230</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
@@ -2910,7 +3272,7 @@
         <v>12475</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
@@ -2927,7 +3289,7 @@
         <v>291484</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
         <v>99</v>
       </c>
@@ -2944,7 +3306,7 @@
         <v>10298</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
         <v>101</v>
       </c>
@@ -2961,7 +3323,7 @@
         <v>10310</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
         <v>102</v>
       </c>
@@ -2977,8 +3339,14 @@
       <c r="E59" s="2">
         <v>129875</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
         <v>105</v>
       </c>
@@ -2994,8 +3362,14 @@
       <c r="E60" s="2">
         <v>108098</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
         <v>106</v>
       </c>
@@ -3011,8 +3385,14 @@
       <c r="E61" s="2">
         <v>129951</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -3028,8 +3408,14 @@
       <c r="E62" s="2">
         <v>130310</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
         <v>108</v>
       </c>
@@ -3045,8 +3431,14 @@
       <c r="E63" s="2">
         <v>130308</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
         <v>109</v>
       </c>
@@ -3062,8 +3454,14 @@
       <c r="E64" s="2">
         <v>130309</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
         <v>110</v>
       </c>
@@ -3079,8 +3477,14 @@
       <c r="E65" s="2">
         <v>536079</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
         <v>111</v>
       </c>
@@ -3097,7 +3501,7 @@
         <v>329641</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
         <v>113</v>
       </c>
@@ -3113,8 +3517,14 @@
       <c r="E67" s="2">
         <v>11137</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1" t="s">
         <v>116</v>
       </c>
@@ -3130,8 +3540,14 @@
       <c r="E68" s="2">
         <v>290028</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1" t="s">
         <v>118</v>
       </c>
@@ -3147,8 +3563,14 @@
       <c r="E69" s="2">
         <v>277944</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
         <v>119</v>
       </c>
@@ -3164,8 +3586,14 @@
       <c r="E70" s="2">
         <v>31631</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
         <v>120</v>
       </c>
@@ -3182,7 +3610,7 @@
         <v>10359</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
         <v>122</v>
       </c>
@@ -3199,7 +3627,7 @@
         <v>11676</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:7">
       <c r="A73" s="1" t="s">
         <v>125</v>
       </c>
@@ -3216,7 +3644,7 @@
         <v>11709</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
         <v>126</v>
       </c>
@@ -3232,8 +3660,14 @@
       <c r="E74" s="2">
         <v>162145</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1" t="s">
         <v>129</v>
       </c>
@@ -3250,7 +3684,7 @@
         <v>10580</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:7">
       <c r="A76" s="1" t="s">
         <v>132</v>
       </c>
@@ -3267,7 +3701,7 @@
         <v>333760</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:7">
       <c r="A77" s="1" t="s">
         <v>133</v>
       </c>
@@ -3284,7 +3718,7 @@
         <v>333761</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
         <v>134</v>
       </c>
@@ -3301,7 +3735,7 @@
         <v>337044</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
         <v>135</v>
       </c>
@@ -3318,7 +3752,7 @@
         <v>10585</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
         <v>136</v>
       </c>
@@ -3607,7 +4041,7 @@
         <v>333767</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
         <v>153</v>
       </c>
@@ -3624,7 +4058,7 @@
         <v>37119</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
         <v>154</v>
       </c>
@@ -3641,7 +4075,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
         <v>155</v>
       </c>
@@ -3658,7 +4092,7 @@
         <v>37121</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
         <v>156</v>
       </c>
@@ -3675,7 +4109,7 @@
         <v>39457</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
         <v>157</v>
       </c>
@@ -3692,7 +4126,7 @@
         <v>51033</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
         <v>158</v>
       </c>
@@ -3709,7 +4143,7 @@
         <v>129724</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
         <v>159</v>
       </c>
@@ -3725,8 +4159,14 @@
       <c r="E103" s="2">
         <v>12730</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
         <v>161</v>
       </c>
@@ -3742,8 +4182,14 @@
       <c r="E104" s="2">
         <v>2560525</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
         <v>163</v>
       </c>
@@ -3759,8 +4205,14 @@
       <c r="E105" s="2">
         <v>11216</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
         <v>164</v>
       </c>
@@ -3776,8 +4228,14 @@
       <c r="E106" s="2">
         <v>2560526</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="1" t="s">
         <v>165</v>
       </c>
@@ -3793,8 +4251,14 @@
       <c r="E107" s="2">
         <v>1803956</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" s="1" t="s">
         <v>167</v>
       </c>
@@ -3811,7 +4275,7 @@
         <v>10798</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:7">
       <c r="A109" s="1" t="s">
         <v>169</v>
       </c>
@@ -3828,7 +4292,7 @@
         <v>746830</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
         <v>171</v>
       </c>
@@ -3845,7 +4309,7 @@
         <v>746831</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
         <v>172</v>
       </c>
@@ -3862,7 +4326,7 @@
         <v>943908</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:7">
       <c r="A112" s="1" t="s">
         <v>174</v>
       </c>
@@ -3878,8 +4342,14 @@
       <c r="E112" s="2">
         <v>208893</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1" t="s">
         <v>176</v>
       </c>
@@ -3895,8 +4365,14 @@
       <c r="E113" s="2">
         <v>208895</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="1" t="s">
         <v>177</v>
       </c>
@@ -3912,8 +4388,14 @@
       <c r="E114" s="2">
         <v>11320</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" s="1" t="s">
         <v>179</v>
       </c>
@@ -3929,8 +4411,14 @@
       <c r="E115" s="2">
         <v>352770</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" s="1" t="s">
         <v>180</v>
       </c>
@@ -3946,8 +4434,14 @@
       <c r="E116" s="2">
         <v>102801</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="1" t="s">
         <v>181</v>
       </c>
@@ -3963,8 +4457,14 @@
       <c r="E117" s="2">
         <v>286285</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" s="1" t="s">
         <v>182</v>
       </c>
@@ -3980,8 +4480,14 @@
       <c r="E118" s="2">
         <v>114727</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="1" t="s">
         <v>183</v>
       </c>
@@ -3997,8 +4503,14 @@
       <c r="E119" s="2">
         <v>36420</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" s="1" t="s">
         <v>184</v>
       </c>
@@ -4014,8 +4526,14 @@
       <c r="E120" s="2">
         <v>641501</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" s="1" t="s">
         <v>185</v>
       </c>
@@ -4031,8 +4549,14 @@
       <c r="E121" s="2">
         <v>114728</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" s="1" t="s">
         <v>186</v>
       </c>
@@ -4048,8 +4572,14 @@
       <c r="E122" s="2">
         <v>114729</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123" s="1" t="s">
         <v>187</v>
       </c>
@@ -4065,8 +4595,14 @@
       <c r="E123" s="2">
         <v>119210</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124" s="1" t="s">
         <v>188</v>
       </c>
@@ -4082,8 +4618,14 @@
       <c r="E124" s="2">
         <v>219633</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125" s="1" t="s">
         <v>189</v>
       </c>
@@ -4099,8 +4641,14 @@
       <c r="E125" s="2">
         <v>502056</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126" s="1" t="s">
         <v>190</v>
       </c>
@@ -4116,8 +4664,14 @@
       <c r="E126" s="2">
         <v>293090</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" s="1" t="s">
         <v>191</v>
       </c>
@@ -4133,8 +4687,14 @@
       <c r="E127" s="2">
         <v>102793</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128" s="1" t="s">
         <v>192</v>
       </c>
@@ -4150,8 +4710,14 @@
       <c r="E128" s="2">
         <v>329376</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
       <c r="A129" s="1" t="s">
         <v>193</v>
       </c>
@@ -4167,8 +4733,14 @@
       <c r="E129" s="2">
         <v>232441</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
       <c r="A130" s="1" t="s">
         <v>194</v>
       </c>
@@ -4184,8 +4756,14 @@
       <c r="E130" s="2">
         <v>119212</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
       <c r="A131" s="1" t="s">
         <v>195</v>
       </c>
@@ -4201,8 +4779,14 @@
       <c r="E131" s="2">
         <v>119214</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
       <c r="A132" s="1" t="s">
         <v>196</v>
       </c>
@@ -4218,8 +4802,14 @@
       <c r="E132" s="2">
         <v>119215</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
       <c r="A133" s="1" t="s">
         <v>197</v>
       </c>
@@ -4235,8 +4825,14 @@
       <c r="E133" s="2">
         <v>325678</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134" s="1" t="s">
         <v>198</v>
       </c>
@@ -4252,8 +4848,14 @@
       <c r="E134" s="2">
         <v>119218</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" s="1" t="s">
         <v>199</v>
       </c>
@@ -4269,8 +4871,14 @@
       <c r="E135" s="2">
         <v>333278</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
       <c r="A136" s="1" t="s">
         <v>200</v>
       </c>
@@ -4286,8 +4894,14 @@
       <c r="E136" s="2">
         <v>102796</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
       <c r="A137" s="1" t="s">
         <v>201</v>
       </c>
@@ -4303,8 +4917,14 @@
       <c r="E137" s="2">
         <v>11520</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
       <c r="A138" s="1" t="s">
         <v>203</v>
       </c>
@@ -4320,8 +4940,14 @@
       <c r="E138" s="2">
         <v>416672</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
       <c r="A139" s="1" t="s">
         <v>204</v>
       </c>
@@ -4337,8 +4963,14 @@
       <c r="E139" s="2">
         <v>416674</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
       <c r="A140" s="1" t="s">
         <v>205</v>
       </c>
@@ -4354,8 +4986,14 @@
       <c r="E140" s="2">
         <v>11552</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
       <c r="A141" s="1" t="s">
         <v>207</v>
       </c>
@@ -4371,8 +5009,14 @@
       <c r="E141" s="2">
         <v>42097</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
       <c r="A142" s="1" t="s">
         <v>208</v>
       </c>
@@ -4388,8 +5032,14 @@
       <c r="E142" s="2">
         <v>261204</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
       <c r="A143" s="1" t="s">
         <v>209</v>
       </c>
@@ -4405,8 +5055,14 @@
       <c r="E143" s="2">
         <v>35511</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
       <c r="A144" s="1" t="s">
         <v>210</v>
       </c>
@@ -4422,8 +5078,14 @@
       <c r="E144" s="2">
         <v>11072</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
       <c r="A145" s="1" t="s">
         <v>211</v>
       </c>
@@ -4440,7 +5102,7 @@
         <v>10632</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:7">
       <c r="A146" s="1" t="s">
         <v>212</v>
       </c>
@@ -4456,8 +5118,14 @@
       <c r="E146" s="2">
         <v>2169991</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
       <c r="A147" s="1" t="s">
         <v>213</v>
       </c>
@@ -4473,8 +5141,14 @@
       <c r="E147" s="2">
         <v>430511</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
       <c r="A148" s="1" t="s">
         <v>214</v>
       </c>
@@ -4491,7 +5165,7 @@
         <v>1891764</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:7">
       <c r="A149" s="1" t="s">
         <v>215</v>
       </c>
@@ -4507,8 +5181,14 @@
       <c r="E149" s="2">
         <v>33743</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
       <c r="A150" s="1" t="s">
         <v>216</v>
       </c>
@@ -4524,8 +5204,14 @@
       <c r="E150" s="2">
         <v>11577</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
       <c r="A151" s="1" t="s">
         <v>217</v>
       </c>
@@ -4542,7 +5228,7 @@
         <v>38766</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:7">
       <c r="A152" s="1" t="s">
         <v>218</v>
       </c>
@@ -4558,8 +5244,14 @@
       <c r="E152" s="2">
         <v>3052489</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
       <c r="A153" s="1" t="s">
         <v>219</v>
       </c>
@@ -4575,8 +5267,14 @@
       <c r="E153" s="2">
         <v>2971765</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
       <c r="A154" s="1" t="s">
         <v>220</v>
       </c>
@@ -4592,8 +5290,14 @@
       <c r="E154" s="2">
         <v>3052310</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
       <c r="A155" s="1" t="s">
         <v>221</v>
       </c>
@@ -4610,7 +5314,7 @@
         <v>1965344</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:7">
       <c r="A156" s="1" t="s">
         <v>222</v>
       </c>
@@ -4626,8 +5330,14 @@
       <c r="E156" s="2">
         <v>3052148</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157" s="1" t="s">
         <v>224</v>
       </c>
@@ -4643,8 +5353,14 @@
       <c r="E157" s="2">
         <v>3052314</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
       <c r="A158" s="1" t="s">
         <v>225</v>
       </c>
@@ -4660,8 +5376,14 @@
       <c r="E158" s="2">
         <v>3052484</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G158" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
       <c r="A159" s="1" t="s">
         <v>226</v>
       </c>
@@ -4677,8 +5399,14 @@
       <c r="E159" s="2">
         <v>3052303</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="F159" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G159" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
       <c r="A160" s="1" t="s">
         <v>227</v>
       </c>
@@ -4694,8 +5422,14 @@
       <c r="E160" s="2">
         <v>3052317</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G160" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
       <c r="A161" s="1" t="s">
         <v>228</v>
       </c>
@@ -4712,7 +5446,7 @@
         <v>1239565</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:7">
       <c r="A162" s="1" t="s">
         <v>231</v>
       </c>
@@ -4729,7 +5463,7 @@
         <v>1239570</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:7">
       <c r="A163" s="1" t="s">
         <v>232</v>
       </c>
@@ -4746,7 +5480,7 @@
         <v>1239572</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:7">
       <c r="A164" s="1" t="s">
         <v>233</v>
       </c>
@@ -4763,7 +5497,7 @@
         <v>1239573</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:7">
       <c r="A165" s="1" t="s">
         <v>234</v>
       </c>
@@ -4779,8 +5513,14 @@
       <c r="E165" s="2">
         <v>238817</v>
       </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="F165" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G165" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
       <c r="A166" s="1" t="s">
         <v>235</v>
       </c>
@@ -4796,8 +5536,14 @@
       <c r="E166" s="2">
         <v>1708253</v>
       </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="F166" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G166" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
       <c r="A167" s="1" t="s">
         <v>237</v>
       </c>
@@ -4813,8 +5559,14 @@
       <c r="E167" s="2">
         <v>59301</v>
       </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="F167" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
       <c r="A168" s="1" t="s">
         <v>238</v>
       </c>
@@ -4830,8 +5582,14 @@
       <c r="E168" s="2">
         <v>11234</v>
       </c>
-    </row>
-    <row r="169" spans="1:5">
+      <c r="F168" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
       <c r="A169" s="1" t="s">
         <v>240</v>
       </c>
@@ -4847,8 +5605,14 @@
       <c r="E169" s="2">
         <v>152219</v>
       </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="F169" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
       <c r="A170" s="1" t="s">
         <v>242</v>
       </c>
@@ -4865,7 +5629,7 @@
         <v>493803</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:7">
       <c r="A171" s="1" t="s">
         <v>243</v>
       </c>
@@ -4881,8 +5645,14 @@
       <c r="E171" s="2">
         <v>1335626</v>
       </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="F171" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
       <c r="A172" s="1" t="s">
         <v>244</v>
       </c>
@@ -4898,8 +5668,14 @@
       <c r="E172" s="2">
         <v>1474807</v>
       </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="F172" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
       <c r="A173" s="1" t="s">
         <v>245</v>
       </c>
@@ -4916,7 +5692,7 @@
         <v>12538</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:7">
       <c r="A174" s="1" t="s">
         <v>246</v>
       </c>
@@ -4932,8 +5708,14 @@
       <c r="E174" s="2">
         <v>10244</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="F174" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
       <c r="A175" s="1" t="s">
         <v>249</v>
       </c>
@@ -4949,8 +5731,14 @@
       <c r="E175" s="2">
         <v>2259728</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
+      <c r="F175" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G175" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
       <c r="A176" s="1" t="s">
         <v>250</v>
       </c>
@@ -4966,8 +5754,14 @@
       <c r="E176" s="2">
         <v>47301</v>
       </c>
-    </row>
-    <row r="177" spans="1:5">
+      <c r="F176" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G176" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
       <c r="A177" s="1" t="s">
         <v>251</v>
       </c>
@@ -4983,8 +5777,14 @@
       <c r="E177" s="2">
         <v>2560602</v>
       </c>
-    </row>
-    <row r="178" spans="1:5">
+      <c r="F177" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
       <c r="A178" s="1" t="s">
         <v>252</v>
       </c>
@@ -5000,8 +5800,14 @@
       <c r="E178" s="2">
         <v>11079</v>
       </c>
-    </row>
-    <row r="179" spans="1:5">
+      <c r="F178" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G178" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
       <c r="A179" s="1" t="s">
         <v>253</v>
       </c>
@@ -5018,7 +5824,7 @@
         <v>1203539</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:7">
       <c r="A180" s="1" t="s">
         <v>254</v>
       </c>
@@ -5035,7 +5841,7 @@
         <v>1497391</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:7">
       <c r="A181" s="1" t="s">
         <v>255</v>
       </c>
@@ -5051,8 +5857,14 @@
       <c r="E181" s="2">
         <v>3052225</v>
       </c>
-    </row>
-    <row r="182" spans="1:5">
+      <c r="F181" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
       <c r="A182" s="1" t="s">
         <v>256</v>
       </c>
@@ -5069,7 +5881,7 @@
         <v>142786</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:7">
       <c r="A183" s="1" t="s">
         <v>258</v>
       </c>
@@ -5086,7 +5898,7 @@
         <v>122928</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:7">
       <c r="A184" s="1" t="s">
         <v>259</v>
       </c>
@@ -5103,7 +5915,7 @@
         <v>122929</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:7">
       <c r="A185" s="1" t="s">
         <v>260</v>
       </c>
@@ -5120,7 +5932,7 @@
         <v>262897</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:7">
       <c r="A186" s="1" t="s">
         <v>261</v>
       </c>
@@ -5137,7 +5949,7 @@
         <v>2594528</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:7">
       <c r="A187" s="1" t="s">
         <v>262</v>
       </c>
@@ -5154,7 +5966,7 @@
         <v>2978453</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:7">
       <c r="A188" s="1" t="s">
         <v>263</v>
       </c>
@@ -5170,8 +5982,14 @@
       <c r="E188" s="2">
         <v>12542</v>
       </c>
-    </row>
-    <row r="189" spans="1:5">
+      <c r="F188" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G188" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
       <c r="A189" s="1" t="s">
         <v>264</v>
       </c>
@@ -5187,8 +6005,14 @@
       <c r="E189" s="2">
         <v>2169701</v>
       </c>
-    </row>
-    <row r="190" spans="1:5">
+      <c r="F189" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
       <c r="A190" s="1" t="s">
         <v>265</v>
       </c>
@@ -5204,8 +6028,14 @@
       <c r="E190" s="2">
         <v>118655</v>
       </c>
-    </row>
-    <row r="191" spans="1:5">
+      <c r="F190" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
       <c r="A191" s="1" t="s">
         <v>266</v>
       </c>
@@ -5221,8 +6051,14 @@
       <c r="E191" s="2">
         <v>443627</v>
       </c>
-    </row>
-    <row r="192" spans="1:5">
+      <c r="F191" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="18">
       <c r="A192" s="1" t="s">
         <v>267</v>
       </c>
@@ -5235,9 +6071,17 @@
       <c r="D192" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E192" s="2"/>
-    </row>
-    <row r="193" spans="1:5">
+      <c r="E192" s="4">
+        <v>12080</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
       <c r="A193" s="1" t="s">
         <v>268</v>
       </c>
@@ -5253,8 +6097,14 @@
       <c r="E193" s="2">
         <v>11083</v>
       </c>
-    </row>
-    <row r="194" spans="1:5">
+      <c r="F193" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G193" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7">
       <c r="A194" s="1" t="s">
         <v>269</v>
       </c>
@@ -5270,8 +6120,14 @@
       <c r="E194" s="2">
         <v>11587</v>
       </c>
-    </row>
-    <row r="195" spans="1:5">
+      <c r="F194" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
       <c r="A195" s="1" t="s">
         <v>271</v>
       </c>
@@ -5287,8 +6143,14 @@
       <c r="E195" s="2">
         <v>3052493</v>
       </c>
-    </row>
-    <row r="196" spans="1:5">
+      <c r="F195" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G195" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
       <c r="A196" s="1" t="s">
         <v>272</v>
       </c>
@@ -5305,7 +6167,7 @@
         <v>11292</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:7">
       <c r="A197" s="1" t="s">
         <v>273</v>
       </c>
@@ -5321,8 +6183,14 @@
       <c r="E197" s="2">
         <v>378809</v>
       </c>
-    </row>
-    <row r="198" spans="1:5">
+      <c r="F197" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
       <c r="A198" s="1" t="s">
         <v>274</v>
       </c>
@@ -5338,8 +6206,14 @@
       <c r="E198" s="2">
         <v>186539</v>
       </c>
-    </row>
-    <row r="199" spans="1:5">
+      <c r="F198" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
       <c r="A199" s="1" t="s">
         <v>275</v>
       </c>
@@ -5355,8 +6229,14 @@
       <c r="E199" s="2">
         <v>147711</v>
       </c>
-    </row>
-    <row r="200" spans="1:5">
+      <c r="F199" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
       <c r="A200" s="1" t="s">
         <v>276</v>
       </c>
@@ -5372,8 +6252,14 @@
       <c r="E200" s="2">
         <v>147712</v>
       </c>
-    </row>
-    <row r="201" spans="1:5">
+      <c r="F200" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
       <c r="A201" s="1" t="s">
         <v>277</v>
       </c>
@@ -5389,8 +6275,14 @@
       <c r="E201" s="2">
         <v>463676</v>
       </c>
-    </row>
-    <row r="202" spans="1:5">
+      <c r="F201" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
       <c r="A202" s="1" t="s">
         <v>278</v>
       </c>
@@ -5406,8 +6298,14 @@
       <c r="E202" s="2">
         <v>11588</v>
       </c>
-    </row>
-    <row r="203" spans="1:5">
+      <c r="F202" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
       <c r="A203" s="1" t="s">
         <v>279</v>
       </c>
@@ -5423,8 +6321,14 @@
       <c r="E203" s="2">
         <v>11029</v>
       </c>
-    </row>
-    <row r="204" spans="1:5">
+      <c r="F203" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
       <c r="A204" s="1" t="s">
         <v>280</v>
       </c>
@@ -5441,7 +6345,7 @@
         <v>28875</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:7">
       <c r="A205" s="1" t="s">
         <v>283</v>
       </c>
@@ -5458,7 +6362,7 @@
         <v>28876</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:7">
       <c r="A206" s="1" t="s">
         <v>284</v>
       </c>
@@ -5475,7 +6379,7 @@
         <v>36427</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:7">
       <c r="A207" s="1" t="s">
         <v>285</v>
       </c>
@@ -5492,7 +6396,7 @@
         <v>1348384</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:7">
       <c r="A208" s="1" t="s">
         <v>286</v>
       </c>
@@ -5509,7 +6413,7 @@
         <v>11041</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:7">
       <c r="A209" s="1" t="s">
         <v>289</v>
       </c>
@@ -5525,8 +6429,14 @@
       <c r="E209" s="2">
         <v>2907957</v>
       </c>
-    </row>
-    <row r="210" spans="1:5">
+      <c r="F209" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
       <c r="A210" s="1" t="s">
         <v>290</v>
       </c>
@@ -5542,8 +6452,14 @@
       <c r="E210" s="2">
         <v>1330524</v>
       </c>
-    </row>
-    <row r="211" spans="1:5">
+      <c r="F210" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
       <c r="A211" s="1" t="s">
         <v>292</v>
       </c>
@@ -5559,8 +6475,14 @@
       <c r="E211" s="2">
         <v>28292</v>
       </c>
-    </row>
-    <row r="212" spans="1:5">
+      <c r="F211" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
       <c r="A212" s="1" t="s">
         <v>293</v>
       </c>
@@ -5576,8 +6498,14 @@
       <c r="E212" s="2">
         <v>3052496</v>
       </c>
-    </row>
-    <row r="213" spans="1:5">
+      <c r="F212" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
       <c r="A213" s="1" t="s">
         <v>294</v>
       </c>
@@ -5594,7 +6522,7 @@
         <v>95341</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:7">
       <c r="A214" s="1" t="s">
         <v>295</v>
       </c>
@@ -5610,8 +6538,14 @@
       <c r="E214" s="2">
         <v>11033</v>
       </c>
-    </row>
-    <row r="215" spans="1:5">
+      <c r="F214" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
       <c r="A215" s="1" t="s">
         <v>296</v>
       </c>
@@ -5627,8 +6561,14 @@
       <c r="E215" s="2">
         <v>3052498</v>
       </c>
-    </row>
-    <row r="216" spans="1:5">
+      <c r="F215" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
       <c r="A216" s="1" t="s">
         <v>297</v>
       </c>
@@ -5644,8 +6584,14 @@
       <c r="E216" s="2">
         <v>2901879</v>
       </c>
-    </row>
-    <row r="217" spans="1:5">
+      <c r="F216" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G216" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
       <c r="A217" s="1" t="s">
         <v>298</v>
       </c>
@@ -5661,8 +6607,14 @@
       <c r="E217" s="2">
         <v>2697049</v>
       </c>
-    </row>
-    <row r="218" spans="1:5">
+      <c r="F217" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G217" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
       <c r="A218" s="1" t="s">
         <v>299</v>
       </c>
@@ -5678,8 +6630,14 @@
       <c r="E218" s="2">
         <v>1003835</v>
       </c>
-    </row>
-    <row r="219" spans="1:5">
+      <c r="F218" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G218" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
       <c r="A219" s="1" t="s">
         <v>300</v>
       </c>
@@ -5696,7 +6654,7 @@
         <v>1891767</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:7">
       <c r="A220" s="1" t="s">
         <v>301</v>
       </c>
@@ -5712,8 +6670,14 @@
       <c r="E220" s="2">
         <v>3052499</v>
       </c>
-    </row>
-    <row r="221" spans="1:5">
+      <c r="F220" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G220" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
       <c r="A221" s="1" t="s">
         <v>302</v>
       </c>
@@ -5729,8 +6693,14 @@
       <c r="E221" s="2">
         <v>11034</v>
       </c>
-    </row>
-    <row r="222" spans="1:5">
+      <c r="F221" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
       <c r="A222" s="1" t="s">
         <v>303</v>
       </c>
@@ -5746,8 +6716,14 @@
       <c r="E222" s="2">
         <v>11580</v>
       </c>
-    </row>
-    <row r="223" spans="1:5">
+      <c r="F222" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
       <c r="A223" s="1" t="s">
         <v>304</v>
       </c>
@@ -5763,8 +6739,14 @@
       <c r="E223" s="2">
         <v>1452514</v>
       </c>
-    </row>
-    <row r="224" spans="1:5">
+      <c r="F223" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
       <c r="A224" s="1" t="s">
         <v>305</v>
       </c>
@@ -5780,8 +6762,14 @@
       <c r="E224" s="2">
         <v>11080</v>
       </c>
-    </row>
-    <row r="225" spans="1:5">
+      <c r="F224" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G224" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
       <c r="A225" s="1" t="s">
         <v>306</v>
       </c>
@@ -5798,7 +6786,7 @@
         <v>1277649</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:7">
       <c r="A226" s="1" t="s">
         <v>307</v>
       </c>
@@ -5814,8 +6802,14 @@
       <c r="E226" s="2">
         <v>186540</v>
       </c>
-    </row>
-    <row r="227" spans="1:5">
+      <c r="F226" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G226" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7">
       <c r="A227" s="1" t="s">
         <v>308</v>
       </c>
@@ -5831,8 +6825,14 @@
       <c r="E227" s="2">
         <v>1608084</v>
       </c>
-    </row>
-    <row r="228" spans="1:5">
+      <c r="F227" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G227" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7">
       <c r="A228" s="1" t="s">
         <v>310</v>
       </c>
@@ -5848,8 +6848,14 @@
       <c r="E228" s="2">
         <v>45270</v>
       </c>
-    </row>
-    <row r="229" spans="1:5">
+      <c r="F228" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G228" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
       <c r="A229" s="1" t="s">
         <v>311</v>
       </c>
@@ -5865,8 +6871,14 @@
       <c r="E229" s="2">
         <v>186541</v>
       </c>
-    </row>
-    <row r="230" spans="1:5">
+      <c r="F229" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G229" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
       <c r="A230" s="1" t="s">
         <v>312</v>
       </c>
@@ -5882,8 +6894,14 @@
       <c r="E230" s="2">
         <v>11084</v>
       </c>
-    </row>
-    <row r="231" spans="1:5">
+      <c r="F230" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G230" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
       <c r="A231" s="1" t="s">
         <v>313</v>
       </c>
@@ -5900,7 +6918,7 @@
         <v>68887</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:7">
       <c r="A232" s="1" t="s">
         <v>316</v>
       </c>
@@ -5916,8 +6934,14 @@
       <c r="E232" s="2">
         <v>11590</v>
       </c>
-    </row>
-    <row r="233" spans="1:5">
+      <c r="F232" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
       <c r="A233" s="1" t="s">
         <v>317</v>
       </c>
@@ -5934,7 +6958,7 @@
         <v>862909</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:7">
       <c r="A234" s="1" t="s">
         <v>318</v>
       </c>
@@ -5950,8 +6974,14 @@
       <c r="E234" s="2">
         <v>3052503</v>
       </c>
-    </row>
-    <row r="235" spans="1:5">
+      <c r="F234" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G234" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
       <c r="A235" s="1" t="s">
         <v>319</v>
       </c>
@@ -5967,8 +6997,14 @@
       <c r="E235" s="2">
         <v>64286</v>
       </c>
-    </row>
-    <row r="236" spans="1:5">
+      <c r="F235" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G235" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
       <c r="A236" s="1" t="s">
         <v>320</v>
       </c>
@@ -5985,7 +7021,7 @@
         <v>10335</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:7">
       <c r="A237" s="1" t="s">
         <v>322</v>
       </c>
@@ -6001,8 +7037,14 @@
       <c r="E237" s="2">
         <v>10255</v>
       </c>
-    </row>
-    <row r="238" spans="1:5">
+      <c r="F237" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G237" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
       <c r="A238" s="1" t="s">
         <v>323</v>
       </c>
@@ -6018,8 +7060,14 @@
       <c r="E238" s="2">
         <v>11036</v>
       </c>
-    </row>
-    <row r="239" spans="1:5">
+      <c r="F238" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G238" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
       <c r="A239" s="1" t="s">
         <v>324</v>
       </c>
@@ -6035,8 +7083,14 @@
       <c r="E239" s="2">
         <v>11082</v>
       </c>
-    </row>
-    <row r="240" spans="1:5">
+      <c r="F239" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G239" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
       <c r="A240" s="1" t="s">
         <v>325</v>
       </c>
@@ -6052,8 +7106,14 @@
       <c r="E240" s="2">
         <v>11039</v>
       </c>
-    </row>
-    <row r="241" spans="1:5">
+      <c r="F240" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
       <c r="A241" s="1" t="s">
         <v>326</v>
       </c>
@@ -6070,7 +7130,7 @@
         <v>440266</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:7">
       <c r="A242" s="1" t="s">
         <v>327</v>
       </c>
@@ -6086,8 +7146,14 @@
       <c r="E242" s="2">
         <v>11089</v>
       </c>
-    </row>
-    <row r="243" spans="1:5">
+      <c r="F242" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G242" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
       <c r="A243" s="1" t="s">
         <v>328</v>
       </c>
@@ -6103,14 +7169,21 @@
       <c r="E243" s="2">
         <v>64320</v>
       </c>
+      <c r="F243" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G243" s="2" t="s">
+        <v>339</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E191 F1:G1 E193:E1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Healthy Places Index (HPI) graph generation
</commit_message>
<xml_diff>
--- a/inputs-sequoia/genus_family.xlsx
+++ b/inputs-sequoia/genus_family.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/github/sequoia-dragen/inputs-sequoia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED26313E-2923-FB4D-A33F-E535035BD63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBB106-250B-2846-A701-2275DF337651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="22400" windowHeight="25500" xr2:uid="{AA6A6641-1C50-7D40-AC2E-61500500FA7D}"/>
+    <workbookView xWindow="640" yWindow="500" windowWidth="22400" windowHeight="25500" xr2:uid="{AA6A6641-1C50-7D40-AC2E-61500500FA7D}"/>
   </bookViews>
   <sheets>
     <sheet name="genus_family" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="342">
   <si>
     <t>Reporting_Name</t>
   </si>
@@ -1132,13 +1132,16 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1307,6 +1310,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1650,12 +1660,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2054,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB977FA-EF16-3246-B6EF-5F9C7D78C9B1}">
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="G231" sqref="G231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2063,7 +2074,7 @@
     <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2106,6 +2117,12 @@
       <c r="E2" s="2">
         <v>10804</v>
       </c>
+      <c r="F2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G2" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
@@ -2238,6 +2255,12 @@
       <c r="E8" s="2">
         <v>90961</v>
       </c>
+      <c r="F8" t="s">
+        <v>341</v>
+      </c>
+      <c r="G8" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
@@ -2278,6 +2301,12 @@
       <c r="E10" s="2">
         <v>1891762</v>
       </c>
+      <c r="F10" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
@@ -2364,6 +2393,12 @@
       <c r="E14" s="2">
         <v>565995</v>
       </c>
+      <c r="F14" t="s">
+        <v>341</v>
+      </c>
+      <c r="G14" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -2519,6 +2554,12 @@
       <c r="E21" s="2">
         <v>46839</v>
       </c>
+      <c r="F21" t="s">
+        <v>341</v>
+      </c>
+      <c r="G21" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
@@ -2789,6 +2830,12 @@
       <c r="E33" s="2">
         <v>38767</v>
       </c>
+      <c r="F33" t="s">
+        <v>341</v>
+      </c>
+      <c r="G33" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
@@ -3036,6 +3083,12 @@
       <c r="E44" s="2">
         <v>10376</v>
       </c>
+      <c r="F44" t="s">
+        <v>341</v>
+      </c>
+      <c r="G44" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
@@ -3053,6 +3106,12 @@
       <c r="E45" s="2">
         <v>38768</v>
       </c>
+      <c r="F45" t="s">
+        <v>341</v>
+      </c>
+      <c r="G45" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
@@ -3231,6 +3290,12 @@
       <c r="E53" s="2">
         <v>10407</v>
       </c>
+      <c r="F53" t="s">
+        <v>341</v>
+      </c>
+      <c r="G53" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
@@ -3271,6 +3336,12 @@
       <c r="E55" s="2">
         <v>12475</v>
       </c>
+      <c r="F55" t="s">
+        <v>341</v>
+      </c>
+      <c r="G55" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
@@ -3288,6 +3359,12 @@
       <c r="E56" s="2">
         <v>291484</v>
       </c>
+      <c r="F56" t="s">
+        <v>341</v>
+      </c>
+      <c r="G56" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
@@ -3305,6 +3382,12 @@
       <c r="E57" s="2">
         <v>10298</v>
       </c>
+      <c r="F57" t="s">
+        <v>341</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
@@ -3322,6 +3405,12 @@
       <c r="E58" s="2">
         <v>10310</v>
       </c>
+      <c r="F58" t="s">
+        <v>341</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
@@ -3500,6 +3589,12 @@
       <c r="E66" s="2">
         <v>329641</v>
       </c>
+      <c r="F66" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
@@ -3609,6 +3704,12 @@
       <c r="E71" s="2">
         <v>10359</v>
       </c>
+      <c r="F71" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
@@ -3626,6 +3727,12 @@
       <c r="E72" s="2">
         <v>11676</v>
       </c>
+      <c r="F72" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1" t="s">
@@ -3643,6 +3750,12 @@
       <c r="E73" s="2">
         <v>11709</v>
       </c>
+      <c r="F73" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
@@ -3683,6 +3796,12 @@
       <c r="E75" s="2">
         <v>10580</v>
       </c>
+      <c r="F75" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="1" t="s">
@@ -3700,6 +3819,12 @@
       <c r="E76" s="2">
         <v>333760</v>
       </c>
+      <c r="F76" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1" t="s">
@@ -3717,6 +3842,12 @@
       <c r="E77" s="2">
         <v>333761</v>
       </c>
+      <c r="F77" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
@@ -3734,6 +3865,12 @@
       <c r="E78" s="2">
         <v>337044</v>
       </c>
+      <c r="F78" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
@@ -3751,6 +3888,12 @@
       <c r="E79" s="2">
         <v>10585</v>
       </c>
+      <c r="F79" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
@@ -3768,8 +3911,14 @@
       <c r="E80" s="2">
         <v>10586</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
         <v>137</v>
       </c>
@@ -3785,8 +3934,14 @@
       <c r="E81" s="2">
         <v>10587</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1" t="s">
         <v>138</v>
       </c>
@@ -3802,8 +3957,14 @@
       <c r="E82" s="2">
         <v>10588</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1" t="s">
         <v>139</v>
       </c>
@@ -3819,8 +3980,14 @@
       <c r="E83" s="2">
         <v>10615</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
         <v>140</v>
       </c>
@@ -3836,8 +4003,14 @@
       <c r="E84" s="2">
         <v>10590</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
         <v>141</v>
       </c>
@@ -3853,8 +4026,14 @@
       <c r="E85" s="2">
         <v>10591</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
         <v>142</v>
       </c>
@@ -3870,8 +4049,14 @@
       <c r="E86" s="2">
         <v>10592</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
         <v>143</v>
       </c>
@@ -3887,8 +4072,14 @@
       <c r="E87" s="2">
         <v>10593</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
         <v>144</v>
       </c>
@@ -3904,8 +4095,14 @@
       <c r="E88" s="2">
         <v>10595</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
         <v>145</v>
       </c>
@@ -3921,8 +4118,14 @@
       <c r="E89" s="2">
         <v>10618</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
         <v>146</v>
       </c>
@@ -3938,8 +4141,14 @@
       <c r="E90" s="2">
         <v>337050</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
         <v>147</v>
       </c>
@@ -3955,8 +4164,14 @@
       <c r="E91" s="2">
         <v>1671798</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1" t="s">
         <v>148</v>
       </c>
@@ -3972,8 +4187,14 @@
       <c r="E92" s="2">
         <v>10596</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
         <v>149</v>
       </c>
@@ -3989,8 +4210,14 @@
       <c r="E93" s="2">
         <v>10598</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
         <v>150</v>
       </c>
@@ -4006,8 +4233,14 @@
       <c r="E94" s="2">
         <v>37115</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
         <v>151</v>
       </c>
@@ -4023,8 +4256,14 @@
       <c r="E95" s="2">
         <v>333754</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
         <v>152</v>
       </c>
@@ -4039,6 +4278,12 @@
       </c>
       <c r="E96" s="2">
         <v>333767</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -4057,6 +4302,12 @@
       <c r="E97" s="2">
         <v>37119</v>
       </c>
+      <c r="F97" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
@@ -4074,6 +4325,12 @@
       <c r="E98" s="2">
         <v>45240</v>
       </c>
+      <c r="F98" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
@@ -4091,6 +4348,12 @@
       <c r="E99" s="2">
         <v>37121</v>
       </c>
+      <c r="F99" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
@@ -4108,6 +4371,12 @@
       <c r="E100" s="2">
         <v>39457</v>
       </c>
+      <c r="F100" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
@@ -4125,6 +4394,12 @@
       <c r="E101" s="2">
         <v>51033</v>
       </c>
+      <c r="F101" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
@@ -4142,6 +4417,12 @@
       <c r="E102" s="2">
         <v>129724</v>
       </c>
+      <c r="F102" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
@@ -4274,6 +4555,12 @@
       <c r="E108" s="2">
         <v>10798</v>
       </c>
+      <c r="F108" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="1" t="s">
@@ -4291,6 +4578,12 @@
       <c r="E109" s="2">
         <v>746830</v>
       </c>
+      <c r="F109" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
@@ -4308,6 +4601,12 @@
       <c r="E110" s="2">
         <v>746831</v>
       </c>
+      <c r="F110" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
@@ -4325,6 +4624,12 @@
       <c r="E111" s="2">
         <v>943908</v>
       </c>
+      <c r="F111" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="1" t="s">
@@ -5101,6 +5406,12 @@
       <c r="E145" s="2">
         <v>10632</v>
       </c>
+      <c r="F145" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G145" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="1" t="s">
@@ -5164,6 +5475,12 @@
       <c r="E148" s="2">
         <v>1891764</v>
       </c>
+      <c r="F148" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G148" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="1" t="s">
@@ -5227,6 +5544,12 @@
       <c r="E151" s="2">
         <v>38766</v>
       </c>
+      <c r="F151" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G151" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="1" t="s">
@@ -5313,6 +5636,12 @@
       <c r="E155" s="2">
         <v>1965344</v>
       </c>
+      <c r="F155" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G155" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="1" t="s">
@@ -5445,6 +5774,12 @@
       <c r="E161" s="2">
         <v>1239565</v>
       </c>
+      <c r="F161" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="1" t="s">
@@ -5462,6 +5797,12 @@
       <c r="E162" s="2">
         <v>1239570</v>
       </c>
+      <c r="F162" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G162" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="1" t="s">
@@ -5479,6 +5820,12 @@
       <c r="E163" s="2">
         <v>1239572</v>
       </c>
+      <c r="F163" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G163" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="1" t="s">
@@ -5496,6 +5843,12 @@
       <c r="E164" s="2">
         <v>1239573</v>
       </c>
+      <c r="F164" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G164" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="1" t="s">
@@ -5628,6 +5981,12 @@
       <c r="E170" s="2">
         <v>493803</v>
       </c>
+      <c r="F170" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G170" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="171" spans="1:7">
       <c r="A171" s="1" t="s">
@@ -5691,6 +6050,12 @@
       <c r="E173" s="2">
         <v>12538</v>
       </c>
+      <c r="F173" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G173" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="174" spans="1:7">
       <c r="A174" s="1" t="s">
@@ -5823,6 +6188,12 @@
       <c r="E179" s="2">
         <v>1203539</v>
       </c>
+      <c r="F179" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G179" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="180" spans="1:7">
       <c r="A180" s="1" t="s">
@@ -5840,6 +6211,12 @@
       <c r="E180" s="2">
         <v>1497391</v>
       </c>
+      <c r="F180" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G180" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="181" spans="1:7">
       <c r="A181" s="1" t="s">
@@ -5880,6 +6257,12 @@
       <c r="E182" s="2">
         <v>142786</v>
       </c>
+      <c r="F182" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G182" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" s="1" t="s">
@@ -5897,6 +6280,12 @@
       <c r="E183" s="2">
         <v>122928</v>
       </c>
+      <c r="F183" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G183" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="1" t="s">
@@ -5914,6 +6303,12 @@
       <c r="E184" s="2">
         <v>122929</v>
       </c>
+      <c r="F184" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G184" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="185" spans="1:7">
       <c r="A185" s="1" t="s">
@@ -5931,6 +6326,12 @@
       <c r="E185" s="2">
         <v>262897</v>
       </c>
+      <c r="F185" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G185" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="1" t="s">
@@ -5948,6 +6349,12 @@
       <c r="E186" s="2">
         <v>2594528</v>
       </c>
+      <c r="F186" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G186" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" s="1" t="s">
@@ -5965,6 +6372,12 @@
       <c r="E187" s="2">
         <v>2978453</v>
       </c>
+      <c r="F187" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G187" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="188" spans="1:7">
       <c r="A188" s="1" t="s">
@@ -6166,6 +6579,12 @@
       <c r="E196" s="2">
         <v>11292</v>
       </c>
+      <c r="F196" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G196" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="197" spans="1:7">
       <c r="A197" s="1" t="s">
@@ -6344,6 +6763,12 @@
       <c r="E204" s="2">
         <v>28875</v>
       </c>
+      <c r="F204" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G204" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="205" spans="1:7">
       <c r="A205" s="1" t="s">
@@ -6361,6 +6786,12 @@
       <c r="E205" s="2">
         <v>28876</v>
       </c>
+      <c r="F205" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G205" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="1" t="s">
@@ -6378,6 +6809,12 @@
       <c r="E206" s="2">
         <v>36427</v>
       </c>
+      <c r="F206" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G206" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="1" t="s">
@@ -6395,6 +6832,12 @@
       <c r="E207" s="2">
         <v>1348384</v>
       </c>
+      <c r="F207" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G207" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="1" t="s">
@@ -6412,6 +6855,12 @@
       <c r="E208" s="2">
         <v>11041</v>
       </c>
+      <c r="F208" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G208" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="1" t="s">
@@ -6521,6 +6970,12 @@
       <c r="E213" s="2">
         <v>95341</v>
       </c>
+      <c r="F213" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G213" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="214" spans="1:7">
       <c r="A214" s="1" t="s">
@@ -6653,6 +7108,12 @@
       <c r="E219" s="2">
         <v>1891767</v>
       </c>
+      <c r="F219" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G219" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="220" spans="1:7">
       <c r="A220" s="1" t="s">
@@ -6785,6 +7246,12 @@
       <c r="E225" s="2">
         <v>1277649</v>
       </c>
+      <c r="F225" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G225" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="1" t="s">
@@ -6917,6 +7384,12 @@
       <c r="E231" s="2">
         <v>68887</v>
       </c>
+      <c r="F231" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G231" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" s="1" t="s">
@@ -6957,6 +7430,12 @@
       <c r="E233" s="2">
         <v>862909</v>
       </c>
+      <c r="F233" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G233" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" s="1" t="s">
@@ -7020,6 +7499,12 @@
       <c r="E236" s="2">
         <v>10335</v>
       </c>
+      <c r="F236" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G236" s="5" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="237" spans="1:7">
       <c r="A237" s="1" t="s">
@@ -7128,6 +7613,12 @@
       </c>
       <c r="E241" s="2">
         <v>440266</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G241" s="5" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="242" spans="1:7">

</xml_diff>

<commit_message>
Fixed genus consolidation and export to json
</commit_message>
<xml_diff>
--- a/inputs-sequoia/genus_family.xlsx
+++ b/inputs-sequoia/genus_family.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/github/sequoia-dragen/inputs-sequoia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBB106-250B-2846-A701-2275DF337651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EDD146-3E73-A04B-9258-AC94B4FA6413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="22400" windowHeight="25500" xr2:uid="{AA6A6641-1C50-7D40-AC2E-61500500FA7D}"/>
   </bookViews>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB977FA-EF16-3246-B6EF-5F9C7D78C9B1}">
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="G231" sqref="G231"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>